<commit_message>
Q3 third revision update
</commit_message>
<xml_diff>
--- a/results/12-2021/12-2021_comparison_deflators.xlsx
+++ b/results/12-2021/12-2021_comparison_deflators.xlsx
@@ -524,7 +524,7 @@
         <v>0.0158</v>
       </c>
       <c r="D2" t="n">
-        <v>0.013</v>
+        <v>0.0131</v>
       </c>
       <c r="E2" t="n">
         <v>0.0043</v>
@@ -647,13 +647,13 @@
         <v>0.0215</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0648</v>
+        <v>-0.0798</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.2132</v>
+        <v>-0.0817</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.2486</v>
+        <v>-0.3785</v>
       </c>
       <c r="G5" t="n">
         <v>-0.0856</v>
@@ -688,7 +688,7 @@
         <v>-0.024</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.0302</v>
+        <v>-0.0259</v>
       </c>
       <c r="E6" t="n">
         <v>-0.0242</v>
@@ -715,7 +715,7 @@
         <v>-0.0568</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.0441</v>
+        <v>-0.0442</v>
       </c>
     </row>
     <row r="7">
@@ -729,16 +729,16 @@
         <v>-0.2563</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.1232</v>
+        <v>-0.124</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.1269</v>
+        <v>-0.1277</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0545</v>
+        <v>0.0537</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1495</v>
+        <v>0.1487</v>
       </c>
       <c r="H7" t="n">
         <v>0.0065</v>
@@ -770,31 +770,31 @@
         <v>-0.3402</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.3036</v>
+        <v>-0.2996</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.3109</v>
+        <v>-0.3096</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.3433</v>
+        <v>-0.3441</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.6567</v>
+        <v>-0.6561</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.5969</v>
+        <v>-0.5964</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.3785</v>
+        <v>-0.378</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.1511</v>
+        <v>-0.1506</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.0484</v>
+        <v>-0.0479</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0214</v>
+        <v>0.0201</v>
       </c>
       <c r="M8" t="n">
         <v>0.0132</v>
@@ -814,31 +814,31 @@
         <v>0.0448</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0203</v>
+        <v>0.0661</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.007</v>
+        <v>-0.0202</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.0063</v>
+        <v>-0.0066</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.1352</v>
+        <v>-0.151</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.0761</v>
+        <v>-0.0763</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.044</v>
+        <v>-0.0441</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0496</v>
+        <v>-0.0498</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.0213</v>
+        <v>-0.0215</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.0315</v>
+        <v>-0.0316</v>
       </c>
     </row>
     <row r="10">
@@ -855,10 +855,10 @@
         <v>0.1381</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2462</v>
+        <v>0.2461</v>
       </c>
       <c r="F10" t="n">
-        <v>0.2121</v>
+        <v>0.212</v>
       </c>
       <c r="G10" t="n">
         <v>0.1649</v>
@@ -893,7 +893,7 @@
         <v>0.0102</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0117</v>
+        <v>0.0123</v>
       </c>
       <c r="E11" t="n">
         <v>0.005</v>
@@ -934,22 +934,22 @@
         <v>-0.1684</v>
       </c>
       <c r="D12" t="n">
-        <v>0.013</v>
+        <v>0.0119</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5055</v>
+        <v>0.5091</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.7273</v>
+        <v>-0.7283</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0803</v>
+        <v>0.0792</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.7728</v>
+        <v>-0.7729</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.5601</v>
+        <v>-0.5649</v>
       </c>
       <c r="J12" t="n">
         <v>-0.0431</v>
@@ -978,31 +978,31 @@
         <v>0.232</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.1205</v>
+        <v>-0.1017</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.1116</v>
+        <v>-0.1144</v>
       </c>
       <c r="G13" t="n">
-        <v>-0.1283</v>
+        <v>-0.1294</v>
       </c>
       <c r="H13" t="n">
-        <v>-0.1173</v>
+        <v>-0.1183</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.0493</v>
+        <v>-0.0503</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.0435</v>
+        <v>-0.0437</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.6121</v>
+        <v>-0.6123</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.6467</v>
+        <v>-0.6469</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.3036</v>
+        <v>-0.3046</v>
       </c>
     </row>
     <row r="14">
@@ -1016,16 +1016,16 @@
         <v>0.1724</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.925</v>
+        <v>-0.9252</v>
       </c>
       <c r="E14" t="n">
-        <v>-1.1036</v>
+        <v>-1.1031</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.9956</v>
+        <v>-0.9958</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.4848</v>
+        <v>-1.485</v>
       </c>
       <c r="H14" t="n">
         <v>-1.0288</v>
@@ -1037,7 +1037,7 @@
         <v>-0.407</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.3157</v>
+        <v>-0.3158</v>
       </c>
       <c r="L14" t="n">
         <v>-0.1462</v>
@@ -1057,34 +1057,34 @@
         <v>-2.304</v>
       </c>
       <c r="D15" t="n">
-        <v>-2.2916</v>
+        <v>-2.3217</v>
       </c>
       <c r="E15" t="n">
-        <v>-1.756</v>
+        <v>-1.6943</v>
       </c>
       <c r="F15" t="n">
-        <v>-1.8239</v>
+        <v>-1.8474</v>
       </c>
       <c r="G15" t="n">
-        <v>-3.2646</v>
+        <v>-3.2671</v>
       </c>
       <c r="H15" t="n">
-        <v>-2.9059</v>
+        <v>-2.8851</v>
       </c>
       <c r="I15" t="n">
-        <v>-2.1067</v>
+        <v>-2.1119</v>
       </c>
       <c r="J15" t="n">
-        <v>-1.9078</v>
+        <v>-1.9074</v>
       </c>
       <c r="K15" t="n">
-        <v>-3.0361</v>
+        <v>-3.0357</v>
       </c>
       <c r="L15" t="n">
-        <v>-1.2165</v>
+        <v>-1.2197</v>
       </c>
       <c r="M15" t="n">
-        <v>-0.6368</v>
+        <v>-0.6379</v>
       </c>
     </row>
     <row r="16">
@@ -1098,7 +1098,7 @@
         <v>22741</v>
       </c>
       <c r="D16" t="n">
-        <v>23187</v>
+        <v>23202.3</v>
       </c>
       <c r="E16" t="n">
         <v>23786.3</v>
@@ -1139,13 +1139,13 @@
         <v>0.5458</v>
       </c>
       <c r="D17" t="n">
-        <v>0.418</v>
+        <v>0.4181</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.2039</v>
+        <v>-0.0724</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.1816</v>
+        <v>-0.3114</v>
       </c>
       <c r="G17" t="n">
         <v>0.1377</v>
@@ -1224,31 +1224,31 @@
         <v>-0.0489</v>
       </c>
       <c r="E19" t="n">
-        <v>-1.1747</v>
+        <v>-1.1619</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0014</v>
+        <v>-0.0021</v>
       </c>
       <c r="G19" t="n">
         <v>-0.0335</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.0353</v>
+        <v>-0.0395</v>
       </c>
       <c r="I19" t="n">
-        <v>-0.0348</v>
+        <v>-0.0349</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.0224</v>
+        <v>-0.0225</v>
       </c>
       <c r="K19" t="n">
-        <v>-1.0898</v>
+        <v>-1.0899</v>
       </c>
       <c r="L19" t="n">
-        <v>-0.0002</v>
+        <v>-0.0003</v>
       </c>
       <c r="M19" t="n">
-        <v>-0.0002</v>
+        <v>-0.0003</v>
       </c>
     </row>
     <row r="20">
@@ -1262,22 +1262,22 @@
         <v>-0.2711</v>
       </c>
       <c r="D20" t="n">
-        <v>-1.1106</v>
+        <v>-1.1108</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.376</v>
+        <v>-0.3758</v>
       </c>
       <c r="F20" t="n">
         <v>-0.0628</v>
       </c>
       <c r="G20" t="n">
-        <v>-1.0283</v>
+        <v>-1.0284</v>
       </c>
       <c r="H20" t="n">
         <v>-0.0306</v>
       </c>
       <c r="I20" t="n">
-        <v>-0.0205</v>
+        <v>-0.0206</v>
       </c>
       <c r="J20" t="n">
         <v>-0.5396</v>
@@ -1303,13 +1303,13 @@
         <v>-0.7397</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.1273</v>
+        <v>-0.1059</v>
       </c>
       <c r="E21" t="n">
-        <v>0.7385</v>
+        <v>0.5857</v>
       </c>
       <c r="F21" t="n">
-        <v>0.5521</v>
+        <v>0.682</v>
       </c>
       <c r="G21" t="n">
         <v>0.1134</v>
@@ -1344,22 +1344,22 @@
         <v>-0.014</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.0118</v>
+        <v>-0.0141</v>
       </c>
       <c r="E22" t="n">
         <v>-0.027</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.0197</v>
+        <v>-0.0196</v>
       </c>
       <c r="G22" t="n">
         <v>-0.0205</v>
       </c>
       <c r="H22" t="n">
-        <v>-0.02</v>
+        <v>-0.0199</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.0198</v>
+        <v>-0.0197</v>
       </c>
       <c r="J22" t="n">
         <v>-0.022</v>
@@ -1385,19 +1385,19 @@
         <v>0.1964</v>
       </c>
       <c r="D23" t="n">
-        <v>0.1389</v>
+        <v>0.094</v>
       </c>
       <c r="E23" t="n">
-        <v>0.2511</v>
+        <v>0.2513</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0844</v>
+        <v>0.0847</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0062</v>
+        <v>0.0065</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.0118</v>
+        <v>0.0301</v>
       </c>
       <c r="I23" t="n">
         <v>0.0117</v>
@@ -1426,31 +1426,31 @@
         <v>-0.0802</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.0828</v>
+        <v>-0.0787</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.0341</v>
+        <v>-0.0334</v>
       </c>
       <c r="F24" t="n">
-        <v>-0.0357</v>
+        <v>-0.0371</v>
       </c>
       <c r="G24" t="n">
-        <v>-0.1181</v>
+        <v>-0.1178</v>
       </c>
       <c r="H24" t="n">
-        <v>-0.0741</v>
+        <v>-0.0738</v>
       </c>
       <c r="I24" t="n">
-        <v>-0.0799</v>
+        <v>-0.0796</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.0517</v>
+        <v>-0.0514</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.0177</v>
+        <v>-0.0174</v>
       </c>
       <c r="L24" t="n">
-        <v>-0.0083</v>
+        <v>-0.0098</v>
       </c>
       <c r="M24" t="n">
         <v>-0.0185</v>
@@ -1508,7 +1508,7 @@
         <v>155</v>
       </c>
       <c r="D26" t="n">
-        <v>158</v>
+        <v>158.2</v>
       </c>
       <c r="E26" t="n">
         <v>160.1076</v>
@@ -1590,10 +1590,10 @@
         <v>-0.2286</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.2048</v>
+        <v>-0.2049</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.0707</v>
+        <v>-0.0706</v>
       </c>
       <c r="F28" t="n">
         <v>-0.1086</v>
@@ -1611,7 +1611,7 @@
         <v>-0.0379</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.0241</v>
+        <v>-0.0242</v>
       </c>
       <c r="L28" t="n">
         <v>-0.0136</v>
@@ -1631,7 +1631,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="E29" t="n">
         <v>0</v>
@@ -1754,13 +1754,13 @@
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>-0.015</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>0.1315</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>-0.1298</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
@@ -1795,7 +1795,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>0</v>
+        <v>0.0042</v>
       </c>
       <c r="E33" t="n">
         <v>0</v>
@@ -1836,16 +1836,16 @@
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>0</v>
+        <v>-0.0008</v>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>-0.0007</v>
       </c>
       <c r="F34" t="n">
-        <v>-0.0315</v>
+        <v>-0.0323</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.0311</v>
+        <v>-0.0319</v>
       </c>
       <c r="H34" t="n">
         <v>-0.0288</v>
@@ -1877,31 +1877,31 @@
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="E35" t="n">
-        <v>0.0028</v>
+        <v>0.0041</v>
       </c>
       <c r="F35" t="n">
-        <v>0.0027</v>
+        <v>0.002</v>
       </c>
       <c r="G35" t="n">
-        <v>0.0014</v>
+        <v>0.002</v>
       </c>
       <c r="H35" t="n">
-        <v>0.0014</v>
+        <v>0.002</v>
       </c>
       <c r="I35" t="n">
-        <v>0.0013</v>
+        <v>0.0019</v>
       </c>
       <c r="J35" t="n">
-        <v>0.0013</v>
+        <v>0.0018</v>
       </c>
       <c r="K35" t="n">
-        <v>0.0013</v>
+        <v>0.0018</v>
       </c>
       <c r="L35" t="n">
-        <v>0.0012</v>
+        <v>0</v>
       </c>
       <c r="M35" t="n">
         <v>0</v>
@@ -1921,31 +1921,31 @@
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>0.0458</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
+        <v>-0.0132</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>-0.0003</v>
       </c>
       <c r="H36" t="n">
-        <v>0</v>
+        <v>-0.0158</v>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="J36" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="K36" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="L36" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="M36" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
     </row>
     <row r="37">
@@ -1962,7 +1962,7 @@
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
@@ -2000,7 +2000,7 @@
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>0</v>
+        <v>0.0005</v>
       </c>
       <c r="E38" t="n">
         <v>0</v>
@@ -2041,22 +2041,22 @@
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.0012</v>
+        <v>-0.0023</v>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>0.0037</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>-0.0011</v>
       </c>
       <c r="G39" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="H39" t="n">
         <v>0.0011</v>
       </c>
       <c r="I39" t="n">
-        <v>0</v>
+        <v>-0.0048</v>
       </c>
       <c r="J39" t="n">
         <v>0</v>
@@ -2085,31 +2085,31 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>0.0188</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>-0.0028</v>
       </c>
       <c r="G40" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="H40" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="J40" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="K40" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="L40" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="M40" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
     </row>
     <row r="41">
@@ -2123,25 +2123,25 @@
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>0.0005</v>
       </c>
       <c r="F41" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="H41" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="J41" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="K41" t="n">
         <v>0</v>
@@ -2164,34 +2164,34 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.0012</v>
+        <v>-0.0313</v>
       </c>
       <c r="E42" t="n">
-        <v>-0.0134</v>
+        <v>0.0483</v>
       </c>
       <c r="F42" t="n">
-        <v>-0.0337</v>
+        <v>-0.0571</v>
       </c>
       <c r="G42" t="n">
-        <v>-0.0376</v>
+        <v>-0.0401</v>
       </c>
       <c r="H42" t="n">
-        <v>-0.0362</v>
+        <v>-0.0154</v>
       </c>
       <c r="I42" t="n">
+        <v>-0.0003</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.0063</v>
+      </c>
+      <c r="K42" t="n">
+        <v>0.0074</v>
+      </c>
+      <c r="L42" t="n">
         <v>0.0049</v>
       </c>
-      <c r="J42" t="n">
-        <v>0.0059</v>
-      </c>
-      <c r="K42" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="L42" t="n">
-        <v>0.008</v>
-      </c>
       <c r="M42" t="n">
-        <v>0.0027</v>
+        <v>0.0016</v>
       </c>
     </row>
     <row r="43">
@@ -2205,7 +2205,7 @@
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>0</v>
+        <v>15.3</v>
       </c>
       <c r="E43" t="n">
         <v>0</v>
@@ -2246,13 +2246,13 @@
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>0.0001</v>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>0.1315</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>-0.1298</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
@@ -2331,16 +2331,16 @@
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>0.0128</v>
       </c>
       <c r="F46" t="n">
-        <v>0</v>
+        <v>-0.0035</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="H46" t="n">
-        <v>0</v>
+        <v>-0.0042</v>
       </c>
       <c r="I46" t="n">
         <v>0</v>
@@ -2369,10 +2369,10 @@
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>0</v>
+        <v>-0.0002</v>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>0.0002</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
@@ -2410,13 +2410,13 @@
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>0</v>
+        <v>0.0214</v>
       </c>
       <c r="E48" t="n">
-        <v>0.0212</v>
+        <v>-0.1316</v>
       </c>
       <c r="F48" t="n">
-        <v>0.0002</v>
+        <v>0.13</v>
       </c>
       <c r="G48" t="n">
         <v>0.0001</v>
@@ -2451,7 +2451,7 @@
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>0</v>
+        <v>-0.0023</v>
       </c>
       <c r="E49" t="n">
         <v>0</v>
@@ -2492,19 +2492,19 @@
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>-0.0449</v>
       </c>
       <c r="E50" t="n">
-        <v>-0.0445</v>
+        <v>-0.0443</v>
       </c>
       <c r="F50" t="n">
-        <v>-0.012</v>
+        <v>-0.0117</v>
       </c>
       <c r="G50" t="n">
-        <v>-0.0119</v>
+        <v>-0.0116</v>
       </c>
       <c r="H50" t="n">
-        <v>-0.0137</v>
+        <v>0.0282</v>
       </c>
       <c r="I50" t="n">
         <v>0.0284</v>
@@ -2533,31 +2533,31 @@
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>0</v>
+        <v>0.0041</v>
       </c>
       <c r="E51" t="n">
-        <v>0.0063</v>
+        <v>0.007</v>
       </c>
       <c r="F51" t="n">
-        <v>0.0062</v>
+        <v>0.0049</v>
       </c>
       <c r="G51" t="n">
-        <v>0.003</v>
+        <v>0.0034</v>
       </c>
       <c r="H51" t="n">
-        <v>0.003</v>
+        <v>0.0033</v>
       </c>
       <c r="I51" t="n">
-        <v>0.003</v>
+        <v>0.0033</v>
       </c>
       <c r="J51" t="n">
-        <v>0.003</v>
+        <v>0.0033</v>
       </c>
       <c r="K51" t="n">
-        <v>0.0029</v>
+        <v>0.0032</v>
       </c>
       <c r="L51" t="n">
-        <v>0.0029</v>
+        <v>0.0014</v>
       </c>
       <c r="M51" t="n">
         <v>0</v>
@@ -2615,7 +2615,7 @@
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E53" t="n">
         <v>0.2024</v>

</xml_diff>